<commit_message>
Aggiunto Preventivo + update
Aggiunto Preventivo, grafici e tabelle orari + sistemato alcune cose
</commit_message>
<xml_diff>
--- a/Piano di Progetto/RiscontroProblemi.xlsx
+++ b/Piano di Progetto/RiscontroProblemi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panoz\Desktop\Marvin-piano_di_progetto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panoz\Documents\GitHub\Marvin\Piano di Progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76A3B82-64B8-4770-9B87-F81B91C5B9FE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574F1AF8-1B90-4C6B-B6A5-4AACA6C56597}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{A9C5908B-2465-420D-9242-B7F005395B64}"/>
   </bookViews>
@@ -132,19 +132,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF3F85B9"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6DAEA"/>
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFD1DEDF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -234,51 +234,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -287,6 +284,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFD1DEDF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -598,7 +600,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,113 +611,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="6"/>
+      <c r="B6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="1" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fine consuntivo + update
</commit_message>
<xml_diff>
--- a/Piano di Progetto/RiscontroProblemi.xlsx
+++ b/Piano di Progetto/RiscontroProblemi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panoz\Documents\GitHub\Marvin\Piano di Progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574F1AF8-1B90-4C6B-B6A5-4AACA6C56597}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC9B6D9-8B00-4836-9FD8-C3A196F6531B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{A9C5908B-2465-420D-9242-B7F005395B64}"/>
   </bookViews>
@@ -248,34 +248,34 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -600,7 +600,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection sqref="A1:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,29 +611,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -642,16 +642,16 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="11" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -662,16 +662,16 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="11" t="s">
+      <c r="A6" s="13"/>
+      <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -682,36 +682,36 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="1" t="s">

</xml_diff>